<commit_message>
update script for dalila
</commit_message>
<xml_diff>
--- a/src/excels/dalila/Epithelial_state_0.2.xlsx
+++ b/src/excels/dalila/Epithelial_state_0.2.xlsx
@@ -12,23 +12,23 @@
     <sheet name="MeV.Fib.4" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="MeV.Fib.6" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="MeV.Endothelial.1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="MeV.Fib_Unknown.8" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="MeV.Endothelial_Injury.4" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="MeV.Immune_doublets.0" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="MeV.FibUnknown.8" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="MeV.EndothelialInjury.4" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="MeV.ImmuneDoublets.0" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="MeV.Fib.1" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="MeV.Endothelial.2" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="MeV.Fib.3" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="MeV.Fib.2" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="MeV.Low_Quality.0" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="MeV.LowQuality.0" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="MeV.ECM.1" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="MeV.ECM.2" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="MeV.ECM.0" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="MeV.Proliferative_Fibr.0" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="MeV.FibProlif.0" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="MeV.Pericytes.0" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="MeV.VLMC.1" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="MeV.Endothelial.3" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="MeV.Epithelial_ECad.0" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="MeV.Fib_CD34.7" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="MeV.EpithelialECad.0" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="MeV.FibCD34.7" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="MeV.SMC.0" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="MeV.Fib.5" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="MeV.VLMC.0" sheetId="25" state="visible" r:id="rId25"/>

</xml_diff>